<commit_message>
ci(labels): add workflow to validate label CSV ordering and remove temp pr_body.md
</commit_message>
<xml_diff>
--- a/docs/GitHub/Colour_Labels_GitHub.xlsx
+++ b/docs/GitHub/Colour_Labels_GitHub.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFB45A8A-E439-4595-B0EB-A6F44AE93D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\P100-Electrical-Agent-Suite\docs\GitHub\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FE97DF3-F16B-4316-A547-82BC7ACD067E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,9 +59,6 @@
     <t>Colour</t>
   </si>
   <si>
-    <t>Solution: Power Platform</t>
-  </si>
-  <si>
     <t>Power Platform</t>
   </si>
   <si>
@@ -75,12 +77,6 @@
     <t>#1F6FEB</t>
   </si>
   <si>
-    <t>Solution: OneDrive</t>
-  </si>
-  <si>
-    <t>OneDrive Container for artifacts falling outside the Power Platform Solution.</t>
-  </si>
-  <si>
     <t>Artifacts (Files, Docs, Reporting, Images)</t>
   </si>
   <si>
@@ -93,9 +89,6 @@
     <t>#0078D4</t>
   </si>
   <si>
-    <t>Agent: EA</t>
-  </si>
-  <si>
     <t>Solution</t>
   </si>
   <si>
@@ -111,24 +104,15 @@
     <t>#B33DC6</t>
   </si>
   <si>
-    <t>Agent: PA</t>
-  </si>
-  <si>
     <t>#6F42C1</t>
   </si>
   <si>
-    <t>Agent: DCA</t>
-  </si>
-  <si>
     <t>DCA →Schema</t>
   </si>
   <si>
     <t>#E85AAD</t>
   </si>
   <si>
-    <t>Schema: Project</t>
-  </si>
-  <si>
     <t>Dataverse: Table</t>
   </si>
   <si>
@@ -144,18 +128,12 @@
     <t>#0B4F6C</t>
   </si>
   <si>
-    <t>Schema: Price Policy</t>
-  </si>
-  <si>
     <t>Price Policy (Root) →Labour Rates (Child) →Labour Roles (Reference) →Columns, Relationships, Business Rules, Keys, Indexes</t>
   </si>
   <si>
     <t>#2D6E2E</t>
   </si>
   <si>
-    <t>Schema: Materials</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
@@ -165,18 +143,12 @@
     <t>#1F9E89</t>
   </si>
   <si>
-    <t>Schema: Task Units</t>
-  </si>
-  <si>
     <t>Task Units (Reference) →Variant Type Master (Reference) →Variant Rules (Child) →Columns, Relationships, Business Rules, Keys, Indexes</t>
   </si>
   <si>
     <t>#2A7F62</t>
   </si>
   <si>
-    <t>Schema: Material Task Units (MTU)</t>
-  </si>
-  <si>
     <t>Association</t>
   </si>
   <si>
@@ -186,45 +158,30 @@
     <t>#0D9488</t>
   </si>
   <si>
-    <t>Schema: Variant Type Master</t>
-  </si>
-  <si>
     <t>Schema: Variant Type Master (Aggregate) →Variant Rules (Child)</t>
   </si>
   <si>
     <t>#10B981</t>
   </si>
   <si>
-    <t>Schema: Circuit Instance</t>
-  </si>
-  <si>
     <t>Circuits Instance (Root)) →Circuit End Point Distribution (Child)→Columns, Relationships, Business Rules, Keys, Indexes</t>
   </si>
   <si>
     <t>#8756FF</t>
   </si>
   <si>
-    <t>Schema: Assembly Template</t>
-  </si>
-  <si>
     <t>Assembly Template (Root) →ACI Materials (Child), ACI Task Units (Child)) →Columns, Relationships, Business Rules, Keys, Indexes</t>
   </si>
   <si>
     <t>#E36209</t>
   </si>
   <si>
-    <t>Schema: Bill of Materials (BOM)</t>
-  </si>
-  <si>
     <t>BOM →Project: Materials →Columns: Relationships, Business Rules, Keys, Indexes</t>
   </si>
   <si>
     <t>#B07219</t>
   </si>
   <si>
-    <t>Platform: Power Automate Flows</t>
-  </si>
-  <si>
     <t>Automation</t>
   </si>
   <si>
@@ -237,9 +194,6 @@
     <t>#00B5D1</t>
   </si>
   <si>
-    <t>Platform: Apps</t>
-  </si>
-  <si>
     <t>Model Driven Application</t>
   </si>
   <si>
@@ -252,9 +206,6 @@
     <t>#8B5CF6</t>
   </si>
   <si>
-    <t>Platform: Security and Governance</t>
-  </si>
-  <si>
     <t>Security</t>
   </si>
   <si>
@@ -267,9 +218,6 @@
     <t>#57606A</t>
   </si>
   <si>
-    <t>Platform: ALM &amp; Extensibility</t>
-  </si>
-  <si>
     <t>Solution Pipeline</t>
   </si>
   <si>
@@ -285,9 +233,6 @@
     <t>#4B5563</t>
   </si>
   <si>
-    <t>Critical</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
@@ -300,21 +245,12 @@
     <t>#D0021B</t>
   </si>
   <si>
-    <t>Important</t>
-  </si>
-  <si>
     <t>#FFB000</t>
   </si>
   <si>
-    <t>Non-Critical</t>
-  </si>
-  <si>
     <t>#00A650</t>
   </si>
   <si>
-    <t>Install</t>
-  </si>
-  <si>
     <t>Areas</t>
   </si>
   <si>
@@ -330,44 +266,119 @@
     <t>#0A84FF</t>
   </si>
   <si>
-    <t>EICR</t>
-  </si>
-  <si>
     <t>#C62828</t>
   </si>
   <si>
-    <t>Emergency Lighting</t>
-  </si>
-  <si>
     <t>#C0CA33</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>#9C27B0</t>
   </si>
   <si>
-    <t>Fault Finding</t>
-  </si>
-  <si>
     <t>#FB8C00</t>
   </si>
   <si>
-    <t>Car Charger</t>
-  </si>
-  <si>
     <t>#00C853</t>
+  </si>
+  <si>
+    <t>1 Solution: Power Platform</t>
+  </si>
+  <si>
+    <t>2 Solution: OneDrive</t>
+  </si>
+  <si>
+    <t>3 Agent: EA</t>
+  </si>
+  <si>
+    <t>4 Agent: PA</t>
+  </si>
+  <si>
+    <t>5 Agent: DCA</t>
+  </si>
+  <si>
+    <t>6 Schema: Project</t>
+  </si>
+  <si>
+    <t>7 Schema: Price Policy</t>
+  </si>
+  <si>
+    <t>8 Schema: Materials</t>
+  </si>
+  <si>
+    <t>9 Schema: Task Units</t>
+  </si>
+  <si>
+    <t>10 Schema: Material Task Units (MTU)</t>
+  </si>
+  <si>
+    <t>11 Schema: Variant Type Master</t>
+  </si>
+  <si>
+    <t>12 Schema: Circuit Instance</t>
+  </si>
+  <si>
+    <t>13 Schema: Assembly Template</t>
+  </si>
+  <si>
+    <t>14 Schema: Bill of Materials (BOM)</t>
+  </si>
+  <si>
+    <t>15 Platform: Power Automate Flows</t>
+  </si>
+  <si>
+    <t>16 Platform: Apps</t>
+  </si>
+  <si>
+    <t>17 Platform: Security and Governance</t>
+  </si>
+  <si>
+    <t>18 Platform: ALM &amp; Extensibility</t>
+  </si>
+  <si>
+    <t>19 Critical</t>
+  </si>
+  <si>
+    <t>20 Important</t>
+  </si>
+  <si>
+    <t>21 Non-Critical</t>
+  </si>
+  <si>
+    <t>22 Install</t>
+  </si>
+  <si>
+    <t>23 EICR</t>
+  </si>
+  <si>
+    <t>24 Emergency Lighting</t>
+  </si>
+  <si>
+    <t>25 Testing</t>
+  </si>
+  <si>
+    <t>26 Fault Finding</t>
+  </si>
+  <si>
+    <t>27 Car Charger</t>
+  </si>
+  <si>
+    <t>OneDrive Container for artifacts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -747,19 +758,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="161.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="161.1328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="83" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -782,589 +795,590 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
         <v>29</v>
       </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" t="s">
         <v>31</v>
       </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E9" t="s">
         <v>33</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
         <v>34</v>
       </c>
-      <c r="F7" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
         <v>35</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
         <v>37</v>
       </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="E11" t="s">
         <v>38</v>
       </c>
-      <c r="F8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
         <v>48</v>
-      </c>
-      <c r="E15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>64</v>
       </c>
       <c r="D16" t="s">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="G17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="G18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="F19" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="F20" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="G20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="F21" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="G21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="F22" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="G22" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="D23" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="F23" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="G23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="D24" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="F24" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="G24" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="D25" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="F25" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="G25" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="F26" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="G26" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="F27" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="G27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>107</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="F28" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="G28" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>